<commit_message>
Post author info balloon added and routes rafactoring
</commit_message>
<xml_diff>
--- a/JS-Frameworks-Self-Evaluation-Protocol-GeorgiPetrov.xlsx
+++ b/JS-Frameworks-Self-Evaluation-Protocol-GeorgiPetrov.xlsx
@@ -642,7 +642,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -740,7 +740,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>18</v>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="C44" s="11">
         <f>SUM(C6:C43)</f>
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D44" s="11">
         <v>370</v>

</xml_diff>

<commit_message>
Likes icon fix and Comment icon added
</commit_message>
<xml_diff>
--- a/JS-Frameworks-Self-Evaluation-Protocol-GeorgiPetrov.xlsx
+++ b/JS-Frameworks-Self-Evaluation-Protocol-GeorgiPetrov.xlsx
@@ -642,7 +642,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -740,7 +740,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>18</v>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="C44" s="11">
         <f>SUM(C6:C43)</f>
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="D44" s="11">
         <v>370</v>

</xml_diff>